<commit_message>
Building everything into a dash web app.
</commit_message>
<xml_diff>
--- a/model/FeatureImportanceDecTree.xlsx
+++ b/model/FeatureImportanceDecTree.xlsx
@@ -598,97 +598,97 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.04184312098989662</v>
+        <v>0.04142577817499517</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00875588793404557</v>
+        <v>0.009119430206315867</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06334367815935198</v>
+        <v>0.06241182299095948</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03307906309301913</v>
+        <v>0.03454793402522253</v>
       </c>
       <c r="F2" t="n">
-        <v>0.008575088932531045</v>
+        <v>0.006746983357423617</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01243340032075724</v>
+        <v>0.01708981157364537</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0002858353369679398</v>
+        <v>0.002754214343031071</v>
       </c>
       <c r="I2" t="n">
-        <v>0.006317354872212987</v>
+        <v>0.007744415193710784</v>
       </c>
       <c r="J2" t="n">
-        <v>0.01216325336935821</v>
+        <v>0.01122666382114934</v>
       </c>
       <c r="K2" t="n">
-        <v>0.02946755781868233</v>
+        <v>0.0293444933506957</v>
       </c>
       <c r="L2" t="n">
-        <v>0.01704633927452997</v>
+        <v>0.01874273300411592</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1177123172350745</v>
+        <v>0.1176529492183252</v>
       </c>
       <c r="N2" t="n">
-        <v>0.03684175686687034</v>
+        <v>0.03598397767625214</v>
       </c>
       <c r="O2" t="n">
-        <v>0.03797619267744323</v>
+        <v>0.03745775885144884</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01617866492110029</v>
+        <v>0.04585725763342981</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.002126583776405964</v>
+        <v>0.001903016537504592</v>
       </c>
       <c r="R2" t="n">
-        <v>0.01409215063605903</v>
+        <v>0.01602069595179173</v>
       </c>
       <c r="S2" t="n">
-        <v>0.01384251584056776</v>
+        <v>0.01585599591014115</v>
       </c>
       <c r="T2" t="n">
-        <v>0.003598709994425547</v>
+        <v>0.003552456232356023</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0008958125469332245</v>
+        <v>0.001103554193260878</v>
       </c>
       <c r="V2" t="n">
-        <v>0.04418616627391148</v>
+        <v>0.003244204487283796</v>
       </c>
       <c r="W2" t="n">
-        <v>0.01901952371311447</v>
+        <v>0.02028403547405648</v>
       </c>
       <c r="X2" t="n">
-        <v>0.008058213958329672</v>
+        <v>0.009219216014908488</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.01275109726500322</v>
+        <v>0.01297439705326808</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.3788225170179231</v>
+        <v>0.3789218855300409</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.004376433639142143</v>
+        <v>0.006435430980247546</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.006689243742726938</v>
+        <v>0.003940864234113369</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.004167700863111269</v>
+        <v>0.0005986726383221138</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.03407385706264014</v>
+        <v>0.03239904666028151</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.007073895833889769</v>
+        <v>0.009558086861860977</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.004206066033975012</v>
+        <v>0.005882217819841569</v>
       </c>
     </row>
     <row r="3">
@@ -698,97 +698,97 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.005667591904527133</v>
+        <v>0.005430693145316895</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0168933738864045</v>
+        <v>0.01733014739952</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01814266599937727</v>
+        <v>0.01460380058829609</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03842251727906617</v>
+        <v>0.04127545179108195</v>
       </c>
       <c r="F3" t="n">
-        <v>0.006967446557897678</v>
+        <v>0.00761940414211925</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02364385745340154</v>
+        <v>0.02690181287263051</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02180760911854852</v>
+        <v>0.01077276703173507</v>
       </c>
       <c r="I3" t="n">
-        <v>0.08863508134461275</v>
+        <v>0.08821409945971646</v>
       </c>
       <c r="J3" t="n">
-        <v>0.06204539584819321</v>
+        <v>0.06012404394019871</v>
       </c>
       <c r="K3" t="n">
-        <v>0.009433945536921702</v>
+        <v>0.009147714987890382</v>
       </c>
       <c r="L3" t="n">
-        <v>0.02744788015352324</v>
+        <v>0.05213656720489655</v>
       </c>
       <c r="M3" t="n">
-        <v>0.01426412323049648</v>
+        <v>0.01658770328325978</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01353192718969602</v>
+        <v>0.01978779799041725</v>
       </c>
       <c r="O3" t="n">
-        <v>0.03235004701332256</v>
+        <v>0.01666765660451682</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01047159050563663</v>
+        <v>0.01868114409032903</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.07783309301731491</v>
+        <v>0.08745644202111151</v>
       </c>
       <c r="R3" t="n">
-        <v>0.008857714621662119</v>
+        <v>0.002255771230602203</v>
       </c>
       <c r="S3" t="n">
-        <v>0.03257109167094199</v>
+        <v>0.0223610516622046</v>
       </c>
       <c r="T3" t="n">
-        <v>0.03557995867322364</v>
+        <v>0.0402277627222782</v>
       </c>
       <c r="U3" t="n">
-        <v>0.003046677816616681</v>
+        <v>0.002155325804836443</v>
       </c>
       <c r="V3" t="n">
-        <v>0.009117739525651446</v>
+        <v>0.009370791832040608</v>
       </c>
       <c r="W3" t="n">
-        <v>0.02692499108785561</v>
+        <v>0.02797177703317714</v>
       </c>
       <c r="X3" t="n">
-        <v>0.01268026748374119</v>
+        <v>0.01227857524741984</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03285818675376351</v>
+        <v>0.03226727897835125</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.01122489494248605</v>
+        <v>0.01011943064000844</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.030399136266528</v>
+        <v>0.03125092536676131</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.08014832838291591</v>
+        <v>0.08521175204645025</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.005454777981659362</v>
+        <v>0.002615321105858613</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.1464804832488897</v>
+        <v>0.1361504474633851</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.04717179449243606</v>
+        <v>0.04333906054307166</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.04992581101268825</v>
+        <v>0.04968748177051784</v>
       </c>
     </row>
     <row r="4">
@@ -798,97 +798,97 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03821856679747125</v>
+        <v>0.0375367542204979</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01123817947307383</v>
+        <v>0.01104799532427805</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01982925685754218</v>
+        <v>0.02124953338710933</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1437502833393466</v>
+        <v>0.1461380717821183</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003351865932975429</v>
+        <v>0.004379993015605014</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01468335459957026</v>
+        <v>0.01444427463941971</v>
       </c>
       <c r="H4" t="n">
-        <v>0.05005767583739493</v>
+        <v>0.05008092761301727</v>
       </c>
       <c r="I4" t="n">
-        <v>0.006724039469231645</v>
+        <v>0.00611441201114897</v>
       </c>
       <c r="J4" t="n">
-        <v>0.006563023098474353</v>
+        <v>0.007412059891202965</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01577193688967351</v>
+        <v>0.01639113273721011</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0545855998278162</v>
+        <v>0.05538818647924072</v>
       </c>
       <c r="M4" t="n">
-        <v>0.04487937106581237</v>
+        <v>0.05000926335668898</v>
       </c>
       <c r="N4" t="n">
-        <v>0.01359497602433297</v>
+        <v>0.01235488903822852</v>
       </c>
       <c r="O4" t="n">
-        <v>0.003386320678624996</v>
+        <v>0.003072695031767502</v>
       </c>
       <c r="P4" t="n">
-        <v>0.009139667978002287</v>
+        <v>0.01278188093152356</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.05396314042721824</v>
+        <v>0.05419485961855384</v>
       </c>
       <c r="R4" t="n">
-        <v>0.006266530796864648</v>
+        <v>0.006561300411942304</v>
       </c>
       <c r="S4" t="n">
-        <v>0.008096303274268106</v>
+        <v>0.001195422787738216</v>
       </c>
       <c r="T4" t="n">
-        <v>0.005207110640838831</v>
+        <v>0.006201744968329247</v>
       </c>
       <c r="U4" t="n">
-        <v>0.005192689518462883</v>
+        <v>0.003847427148078504</v>
       </c>
       <c r="V4" t="n">
-        <v>0.009959747120292501</v>
+        <v>0.009697053459384644</v>
       </c>
       <c r="W4" t="n">
-        <v>0.02075307900807175</v>
+        <v>0.02017929451578506</v>
       </c>
       <c r="X4" t="n">
-        <v>0.0331259930506668</v>
+        <v>0.03399465607717327</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.00421867656382083</v>
+        <v>0.003557322283427295</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.2103376212627979</v>
+        <v>0.2060217991627378</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.03970697859353602</v>
+        <v>0.04147274177975339</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.002514497368281075</v>
+        <v>0.00405944574485724</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.01078931898382368</v>
+        <v>0.009948158276379812</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.03843457922389042</v>
+        <v>0.03818103056963332</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.0347839726532494</v>
+        <v>0.03164705416915764</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.0808756436445741</v>
+        <v>0.08083861956801182</v>
       </c>
     </row>
     <row r="5">
@@ -898,97 +898,97 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0009121786737165237</v>
+        <v>0.003654232166171411</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003700236243034796</v>
+        <v>0.002158544405972808</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01232938003489741</v>
+        <v>0.01183967758953136</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02419859513562524</v>
+        <v>0.01866090832493984</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0151125983461853</v>
+        <v>0.01446280946140693</v>
       </c>
       <c r="G5" t="n">
-        <v>0.004224120466037831</v>
+        <v>0.007229007585270534</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0002876585469485733</v>
+        <v>0.0003810451720702955</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01246779306359055</v>
+        <v>0.01278701192038035</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1417781562101182</v>
+        <v>0.1476211048891866</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1132089708531775</v>
+        <v>0.1089982620909422</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0006988673140411224</v>
+        <v>0.0005195480759701095</v>
       </c>
       <c r="M5" t="n">
-        <v>0.03250752818294517</v>
+        <v>0.05046100159478484</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0309437738784408</v>
+        <v>0.01469944268240226</v>
       </c>
       <c r="O5" t="n">
-        <v>0.007596390630825356</v>
+        <v>0.005796035707624606</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0214558237723858</v>
+        <v>0.01997210143578817</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.01626423484080345</v>
+        <v>0.009595571741369078</v>
       </c>
       <c r="R5" t="n">
-        <v>0.02714654374635692</v>
+        <v>0.02507843072808258</v>
       </c>
       <c r="S5" t="n">
-        <v>0.100471776525073</v>
+        <v>0.06044767317500175</v>
       </c>
       <c r="T5" t="n">
-        <v>0.006592020552498267</v>
+        <v>0.006199195465047543</v>
       </c>
       <c r="U5" t="n">
-        <v>0.01658848305339557</v>
+        <v>0.02335360735967333</v>
       </c>
       <c r="V5" t="n">
-        <v>0.007450118964745988</v>
+        <v>0.01355941691592833</v>
       </c>
       <c r="W5" t="n">
-        <v>0.01524212418706434</v>
+        <v>0.01721846991812657</v>
       </c>
       <c r="X5" t="n">
-        <v>0.2412553087564211</v>
+        <v>0.2411835088666599</v>
       </c>
       <c r="Y5" t="n">
-        <v>9.665590014420999e-06</v>
+        <v>6.318900565257367e-05</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.02916892428992652</v>
+        <v>0.03421501058572696</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.004896028940715025</v>
+        <v>0.002544259671756123</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.001300276607144954</v>
+        <v>0.002345196231393964</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.002196471420554953</v>
+        <v>0.004727319463771576</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.07036453179811362</v>
+        <v>0.06557196696475304</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.02117799142654928</v>
+        <v>0.02104673627157618</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.01845342794865243</v>
+        <v>0.05360971453303842</v>
       </c>
     </row>
     <row r="6">
@@ -998,97 +998,97 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.002021147034419414</v>
+        <v>0.002160616185580105</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03129961646141075</v>
+        <v>0.02885305528827399</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001445605442042811</v>
+        <v>0.004749989247254319</v>
       </c>
       <c r="E6" t="n">
-        <v>0.003830543341542194</v>
+        <v>0.003508283595324904</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02522137808925026</v>
+        <v>0.02134129292158206</v>
       </c>
       <c r="G6" t="n">
-        <v>0.009898813716866526</v>
+        <v>0.009636866492675016</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0005335353240207725</v>
+        <v>2.288868142801144e-05</v>
       </c>
       <c r="I6" t="n">
-        <v>0.008988364768946815</v>
+        <v>0.01205193860758435</v>
       </c>
       <c r="J6" t="n">
-        <v>0.01163631442154262</v>
+        <v>0.01067785276152942</v>
       </c>
       <c r="K6" t="n">
-        <v>0.001745363066028165</v>
+        <v>0.001736406199645091</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0484926904540818</v>
+        <v>0.0522348654203845</v>
       </c>
       <c r="M6" t="n">
-        <v>0.03027290627497071</v>
+        <v>0.02987110892152077</v>
       </c>
       <c r="N6" t="n">
-        <v>0.009521949652177336</v>
+        <v>0.009475843717048736</v>
       </c>
       <c r="O6" t="n">
-        <v>0.00170360594016984</v>
+        <v>0.008091326248291021</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0325661924786265</v>
+        <v>0.04669995423115453</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1042000416697814</v>
+        <v>0.1057454707948054</v>
       </c>
       <c r="R6" t="n">
-        <v>0.01065723854184482</v>
+        <v>0.01219480080115458</v>
       </c>
       <c r="S6" t="n">
-        <v>0.06166734036569844</v>
+        <v>0.06861092574414444</v>
       </c>
       <c r="T6" t="n">
-        <v>0.001705646265436527</v>
+        <v>0.001841006657040083</v>
       </c>
       <c r="U6" t="n">
-        <v>0.01023175192662556</v>
+        <v>0.006958404391208561</v>
       </c>
       <c r="V6" t="n">
-        <v>0.08089449567315382</v>
+        <v>0.07486274267063055</v>
       </c>
       <c r="W6" t="n">
-        <v>0.01910114707811497</v>
+        <v>0.01712233474334489</v>
       </c>
       <c r="X6" t="n">
-        <v>0.0979873651370733</v>
+        <v>0.09800816490071609</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.002279850776846147</v>
+        <v>0.002262070375608591</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.01109194182399309</v>
+        <v>0.008534597867902777</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.009575133620232899</v>
+        <v>0.002335768728363975</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.003075140466423207</v>
+        <v>0.002106293295639031</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.0008708174006042515</v>
+        <v>0.0002615803796677384</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.09452182670394964</v>
+        <v>0.09582973492160531</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.1435392233552354</v>
+        <v>0.1401594763039248</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.12942301272889</v>
+        <v>0.1220543389049664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>